<commit_message>
Toimiva robo (läpi ajettu)
</commit_message>
<xml_diff>
--- a/Laskut yhteenveto/LaskutYhteenveto-2025.04.12.xlsx
+++ b/Laskut yhteenveto/LaskutYhteenveto-2025.04.12.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://konecranes1-my.sharepoint.com/personal/samu_yrttiaho_konecranes_com/Documents/Documents/UiPath/Harkkatyö1/Laskut yhteenveto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarre\Documents\UiPath\DigiLii_harjoitusty-\Laskut yhteenveto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{D1DC54B7-7E2E-4FC2-9D93-AC4D09CBC0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B7E3D20-C70C-4C0D-A318-C3B2B3B69CDA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2908C14-029B-494E-A2EA-9E40CB01E70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="900" windowWidth="14400" windowHeight="8260" firstSheet="1" activeTab="2" xr2:uid="{6C522AF7-2DAC-4D08-B4BD-E50CDF0402DF}"/>
+    <workbookView xWindow="15705" yWindow="8265" windowWidth="17505" windowHeight="12735" activeTab="2" xr2:uid="{EF01687A-0CD1-401C-901D-DA5B80AE9A52}"/>
   </bookViews>
   <sheets>
     <sheet name="Maksetut laskut" sheetId="1" r:id="rId1"/>
@@ -89,7 +89,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-teema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -420,14 +420,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DAD608-AD57-4DA2-8E77-2A5768914D66}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA3A82C-5214-46BA-A1C2-975374438D01}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,14 +444,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D9FB9CB-414D-4DC0-B2E6-2008932390B8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF20AC49-01F0-47E4-8E1C-020B7CAA82DE}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,14 +468,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{199008CF-E55D-41E4-84BF-BD76B3AC7A5E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5204CB68-2969-4071-BEBD-C9D7C46473EA}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>

</xml_diff>